<commit_message>
Fix issue with busco score. Split taxon with 1 proteome and taxon with more proteomes.
</commit_message>
<xml_diff>
--- a/esmecata/Example.xlsx
+++ b/esmecata/Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnaud\Downloads\stage_baptiste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnaud\Downloads\Work_directory\programs\esmecata\esmecata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0C6709F-F6A3-4D44-8007-05E41D00EDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109A89AB-D02A-4F7B-B779-29EE0A1BEAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>observation_name</t>
   </si>
@@ -82,12 +82,18 @@
   </si>
   <si>
     <t>Bacteria;Firmicutes;Clostridia;Clostridiales;Clostridiaceae;Clostridium;unknown species</t>
+  </si>
+  <si>
+    <t>Cluster_8</t>
+  </si>
+  <si>
+    <t>Viruses;Riboviria;Orthornavirae;Kitrinoviricota;Alsuviricetes;Tymovirales;Betaflexiviridae;Trivirinae;Chordovirus;Carrot Ch virus 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,11 +438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,6 +511,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>